<commit_message>
date base functionality added
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -360,7 +360,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E12"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -392,17 +392,6 @@
           <t>Dhaka</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ঢাকা বিশ্ববিদ্যালয়
-সরকারি বিশ্ববিদ্যালয়, ঢাকা, বাংলাদেশ</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ঢাকা কলেজ</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="inlineStr">
@@ -415,17 +404,6 @@
           <t>Saturday</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Saturday Night Live
-স্যাটারডে নাইট লাইভ — টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>saturday</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="inlineStr">
@@ -438,17 +416,6 @@
           <t>Baby</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Baby Monster
-বেবি মনস্টার — মিউজিক্যাল গ্রুপ</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>baby</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="B6" s="2" t="inlineStr">
@@ -461,17 +428,6 @@
           <t>School</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>School 2017
-টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>school</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="inlineStr">
@@ -484,17 +440,6 @@
           <t>Cricket</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>cricket icc
-আন্তর্জাতিক ক্রিকেট কাউন্সিল — ক্রিকেট প্রশাসনিক সংস্থা</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>cricket</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="inlineStr">
@@ -507,16 +452,6 @@
           <t>Momey</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>money cannot bring happiness story</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>money</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="inlineStr">
@@ -529,17 +464,6 @@
           <t>Int</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>inter milan
-ইন্টার মিলান — ফুটবল টীম</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>inter miami vs</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="inlineStr">
@@ -552,17 +476,6 @@
           <t>Look</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>lookism
-লুকিজম — কমিক বই ক্রম</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>look</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="B11" s="2" t="inlineStr">
@@ -575,17 +488,6 @@
           <t>Hello</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Hello Kitty
-কাল্পনিক চরিত্র</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>hello hello</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="B12" s="2" t="inlineStr">
@@ -596,16 +498,6 @@
       <c r="C12" s="2" t="inlineStr">
         <is>
           <t>By</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>বয়স্ক ভাতা অনলাইন আবেদন ২০২৩</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>ব্যাংক</t>
         </is>
       </c>
     </row>
@@ -620,7 +512,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E12"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -652,17 +544,6 @@
           <t>Dhaka</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ঢাকা বিশ্ববিদ্যালয়
-সরকারি বিশ্ববিদ্যালয়, ঢাকা, বাংলাদেশ</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ঢাকা কলেজ</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="inlineStr">
@@ -675,17 +556,6 @@
           <t>Sunday</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>sunday horror special
-সানডে হরর স্পেশাল — টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>sunday</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="inlineStr">
@@ -698,17 +568,6 @@
           <t>Baby</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Baby Monster
-বেবি মনস্টার — মিউজিক্যাল গ্রুপ</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>baby</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="B6" s="2" t="inlineStr">
@@ -721,17 +580,6 @@
           <t>School</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>School 2017
-টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>school</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="inlineStr">
@@ -744,17 +592,6 @@
           <t>Cricket</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>cricket icc
-আন্তর্জাতিক ক্রিকেট কাউন্সিল — ক্রিকেট প্রশাসনিক সংস্থা</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>cricket</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="inlineStr">
@@ -767,16 +604,6 @@
           <t>Momey</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>money cannot bring happiness story</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>money</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="inlineStr">
@@ -789,17 +616,6 @@
           <t>Int</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>inter milan
-ইন্টার মিলান — ফুটবল টীম</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>inter miami vs</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="inlineStr">
@@ -812,17 +628,6 @@
           <t>Look</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>lookism
-লুকিজম — কমিক বই ক্রম</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>look</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="B11" s="2" t="inlineStr">
@@ -835,17 +640,6 @@
           <t>Hello</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Hello Kitty
-কাল্পনিক চরিত্র</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>hello hello</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="B12" s="2" t="inlineStr">
@@ -856,16 +650,6 @@
       <c r="C12" s="2" t="inlineStr">
         <is>
           <t>By</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>বয়স্ক ভাতা অনলাইন আবেদন ২০২৩</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>ব্যাংক</t>
         </is>
       </c>
     </row>
@@ -1050,13 +834,13 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>inter milan
-ইন্টার মিলান — ফুটবল টীম</t>
+          <t>ইন্টার মায়ামি সিএফ
+ফুটবল টীম</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>inter miami vs</t>
+          <t>ইন্টারনেট কি</t>
         </is>
       </c>
     </row>
@@ -1139,7 +923,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E12"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1171,17 +955,6 @@
           <t>Dhaka</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ঢাকা বিশ্ববিদ্যালয়
-সরকারি বিশ্ববিদ্যালয়, ঢাকা, বাংলাদেশ</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ঢাকা কলেজ</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="inlineStr">
@@ -1194,17 +967,6 @@
           <t>Saturday</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Saturday Night Live
-স্যাটারডে নাইট লাইভ — টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>saturday</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="inlineStr">
@@ -1217,17 +979,6 @@
           <t>Baby</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Baby Monster
-বেবি মনস্টার — মিউজিক্যাল গ্রুপ</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>baby</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="B6" s="2" t="inlineStr">
@@ -1240,17 +991,6 @@
           <t>School</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>School 2017
-টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>school</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="inlineStr">
@@ -1263,17 +1003,6 @@
           <t>Cricket</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>cricket icc
-আন্তর্জাতিক ক্রিকেট কাউন্সিল — ক্রিকেট প্রশাসনিক সংস্থা</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>cricket</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="inlineStr">
@@ -1286,16 +1015,6 @@
           <t>Momey</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>money cannot bring happiness story</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>money</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="inlineStr">
@@ -1308,17 +1027,6 @@
           <t>Int</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>inter milan
-ইন্টার মিলান — ফুটবল টীম</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>inter miami vs</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="inlineStr">
@@ -1331,17 +1039,6 @@
           <t>Hubby</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>hubby meaning in bengali
-স্বামী (বাংলা)</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>hubby</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="B11" s="2" t="inlineStr">
@@ -1354,17 +1051,6 @@
           <t>Hello</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Hello Kitty
-কাল্পনিক চরিত্র</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>hello hello</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="B12" s="2" t="inlineStr">
@@ -1375,16 +1061,6 @@
       <c r="C12" s="2" t="inlineStr">
         <is>
           <t>By</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>বয়স্ক ভাতা অনলাইন আবেদন ২০২৩</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>ব্যাংক</t>
         </is>
       </c>
     </row>
@@ -1399,7 +1075,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E12"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1431,17 +1107,6 @@
           <t>Dhaka</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ঢাকা বিশ্ববিদ্যালয়
-সরকারি বিশ্ববিদ্যালয়, ঢাকা, বাংলাদেশ</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ঢাকা কলেজ</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="inlineStr">
@@ -1454,17 +1119,6 @@
           <t>Saturday</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Saturday Night Live
-স্যাটারডে নাইট লাইভ — টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>saturday</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="inlineStr">
@@ -1477,17 +1131,6 @@
           <t>Baby</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Baby Monster
-বেবি মনস্টার — মিউজিক্যাল গ্রুপ</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>baby</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="B6" s="2" t="inlineStr">
@@ -1500,17 +1143,6 @@
           <t>School</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>School 2017
-টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>school</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="inlineStr">
@@ -1523,17 +1155,6 @@
           <t>Cricket</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>cricket icc
-আন্তর্জাতিক ক্রিকেট কাউন্সিল — ক্রিকেট প্রশাসনিক সংস্থা</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>cricket</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="inlineStr">
@@ -1546,16 +1167,6 @@
           <t>Pathao</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>pathao rider helpline number</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>pathao food</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="inlineStr">
@@ -1568,17 +1179,6 @@
           <t>Int</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>inter milan
-ইন্টার মিলান — ফুটবল টীম</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>inter miami vs</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="inlineStr">
@@ -1591,17 +1191,6 @@
           <t>Look</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>lookism
-লুকিজম — কমিক বই ক্রম</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>look</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="B11" s="2" t="inlineStr">
@@ -1614,17 +1203,6 @@
           <t>Hello</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Hello Kitty
-কাল্পনিক চরিত্র</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>hello hello</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="B12" s="2" t="inlineStr">
@@ -1635,16 +1213,6 @@
       <c r="C12" s="2" t="inlineStr">
         <is>
           <t>By</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>বয়স্ক ভাতা অনলাইন আবেদন ২০২৩</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>ব্যাংক</t>
         </is>
       </c>
     </row>
@@ -1659,7 +1227,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E12"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1691,17 +1259,6 @@
           <t>Dhaka</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ঢাকা বিশ্ববিদ্যালয়
-সরকারি বিশ্ববিদ্যালয়, ঢাকা, বাংলাদেশ</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ঢাকা কলেজ</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="inlineStr">
@@ -1714,17 +1271,6 @@
           <t>Saturday</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Saturday Night Live
-স্যাটারডে নাইট লাইভ — টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>saturday</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="inlineStr">
@@ -1737,17 +1283,6 @@
           <t>Baby</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Baby Monster
-বেবি মনস্টার — মিউজিক্যাল গ্রুপ</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>baby</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="B6" s="2" t="inlineStr">
@@ -1760,17 +1295,6 @@
           <t>School</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>School 2017
-টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>school</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="inlineStr">
@@ -1783,17 +1307,6 @@
           <t>Cricket</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>cricket icc
-আন্তর্জাতিক ক্রিকেট কাউন্সিল — ক্রিকেট প্রশাসনিক সংস্থা</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>cricket</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="inlineStr">
@@ -1806,16 +1319,6 @@
           <t>Momey</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>money cannot bring happiness story</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>money</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="inlineStr">
@@ -1828,17 +1331,6 @@
           <t>Int</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>inter milan
-ইন্টার মিলান — ফুটবল টীম</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>inter miami vs</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="inlineStr">
@@ -1851,17 +1343,6 @@
           <t>Goods</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Goods In Motion
-সফ্টওয়্যার কোম্পানি · ঢাকা</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>goods</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="B11" s="2" t="inlineStr">
@@ -1874,17 +1355,6 @@
           <t>Hello</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Hello Kitty
-কাল্পনিক চরিত্র</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>hello hello</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="B12" s="2" t="inlineStr">
@@ -1895,16 +1365,6 @@
       <c r="C12" s="2" t="inlineStr">
         <is>
           <t>By</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>বয়স্ক ভাতা অনলাইন আবেদন ২০২৩</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>ব্যাংক</t>
         </is>
       </c>
     </row>
@@ -1919,7 +1379,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E12"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1957,17 +1417,6 @@
           <t>Dhaka</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ঢাকা বিশ্ববিদ্যালয়
-সরকারি বিশ্ববিদ্যালয়, ঢাকা, বাংলাদেশ</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ঢাকা কলেজ</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="inlineStr">
@@ -1980,17 +1429,6 @@
           <t>Saturday</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Saturday Night Live
-স্যাটারডে নাইট লাইভ — টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>saturday</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="B5" s="2" t="inlineStr">
@@ -2003,17 +1441,6 @@
           <t>Baby</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Baby Monster
-বেবি মনস্টার — মিউজিক্যাল গ্রুপ</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>baby</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="B6" s="2" t="inlineStr">
@@ -2026,17 +1453,6 @@
           <t>School</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>School 2017
-টিভি প্রোগ্রাম</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>school</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="2" t="inlineStr">
@@ -2049,17 +1465,6 @@
           <t>Cricket</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>cricket icc
-আন্তর্জাতিক ক্রিকেট কাউন্সিল — ক্রিকেট প্রশাসনিক সংস্থা</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>cricket</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="B8" s="2" t="inlineStr">
@@ -2072,17 +1477,6 @@
           <t>Geography</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Geography Of Bangladesh
-হারুন রশিদ এর পুস্তক</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>geography</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="B9" s="2" t="inlineStr">
@@ -2095,17 +1489,6 @@
           <t>Int</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>inter milan
-ইন্টার মিলান — ফুটবল টীম</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>inter miami vs</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="inlineStr">
@@ -2118,17 +1501,6 @@
           <t>Look</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>lookism
-লুকিজম — কমিক বই ক্রম</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>look</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="B11" s="2" t="inlineStr">
@@ -2141,17 +1513,6 @@
           <t>Hello</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Hello Kitty
-কাল্পনিক চরিত্র</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>hello hello</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="B12" s="2" t="inlineStr">
@@ -2162,16 +1523,6 @@
       <c r="C12" s="2" t="inlineStr">
         <is>
           <t>By</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>বয়স্ক ভাতা অনলাইন আবেদন ২০২৩</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>ব্যাংক</t>
         </is>
       </c>
     </row>

</xml_diff>